<commit_message>
modified:   stock_analysis.ipynb 	modified:   stock_analysis_final.xlsx
</commit_message>
<xml_diff>
--- a/stock_analysis_final.xlsx
+++ b/stock_analysis_final.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Запасы (дней)</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>Выпустить до:</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -5849,11 +5846,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5869,7 +5866,7 @@
     <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>115</v>
       </c>
@@ -5887,7 +5884,7 @@
       </c>
       <c r="I1" s="31"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>4</v>
       </c>
@@ -5896,7 +5893,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -5917,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
@@ -5926,7 +5923,7 @@
       <c r="D4" s="16"/>
       <c r="E4" s="27"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>26</v>
       </c>
@@ -5947,7 +5944,7 @@
         <v>2022-11-15</v>
       </c>
       <c r="G5" s="33" t="str">
-        <f>IF(H5&gt;0,"•","")</f>
+        <f t="shared" ref="G5:G50" si="0">IF(H5&gt;0,"•","")</f>
         <v>•</v>
       </c>
       <c r="H5" s="34">
@@ -5956,7 +5953,7 @@
       </c>
       <c r="I5" s="31"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>17</v>
       </c>
@@ -5977,7 +5974,7 @@
         <v>2022-11-24</v>
       </c>
       <c r="G6" s="33" t="str">
-        <f>IF(H6&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v>•</v>
       </c>
       <c r="H6" s="34">
@@ -5985,7 +5982,7 @@
         <v>3827</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>30</v>
       </c>
@@ -6006,7 +6003,7 @@
         <v>2022-11-24</v>
       </c>
       <c r="G7" s="33" t="str">
-        <f>IF(H7&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H7" s="34">
@@ -6014,7 +6011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
@@ -6035,7 +6032,7 @@
         <v>2022-11-28</v>
       </c>
       <c r="G8" s="33" t="str">
-        <f>IF(H8&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v>•</v>
       </c>
       <c r="H8" s="34">
@@ -6043,7 +6040,7 @@
         <v>15267</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>22</v>
       </c>
@@ -6064,7 +6061,7 @@
         <v>2022-11-28</v>
       </c>
       <c r="G9" s="33" t="str">
-        <f>IF(H9&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H9" s="34">
@@ -6072,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>34</v>
       </c>
@@ -6093,7 +6090,7 @@
         <v>2022-11-29</v>
       </c>
       <c r="G10" s="33" t="str">
-        <f>IF(H10&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H10" s="34">
@@ -6101,7 +6098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>47</v>
       </c>
@@ -6122,18 +6119,15 @@
         <v>2022-11-29</v>
       </c>
       <c r="G11" s="33" t="str">
-        <f>IF(H11&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v>•</v>
       </c>
       <c r="H11" s="34">
         <f>VLOOKUP(A11,[2]остатки!$B$8:$M$124,12,FALSE)</f>
         <v>21828</v>
       </c>
-      <c r="J11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>35</v>
       </c>
@@ -6154,7 +6148,7 @@
         <v>2022-11-30</v>
       </c>
       <c r="G12" s="33" t="str">
-        <f>IF(H12&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H12" s="34">
@@ -6162,7 +6156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>7</v>
       </c>
@@ -6183,7 +6177,7 @@
         <v>2022-11-30</v>
       </c>
       <c r="G13" s="33" t="str">
-        <f>IF(H13&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v>•</v>
       </c>
       <c r="H13" s="34">
@@ -6191,7 +6185,7 @@
         <v>13875</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>20</v>
       </c>
@@ -6212,7 +6206,7 @@
         <v>2022-12-01</v>
       </c>
       <c r="G14" s="33" t="str">
-        <f>IF(H14&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H14" s="34">
@@ -6220,7 +6214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>13</v>
       </c>
@@ -6241,7 +6235,7 @@
         <v>2022-12-01</v>
       </c>
       <c r="G15" s="33" t="str">
-        <f>IF(H15&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H15" s="34">
@@ -6249,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>14</v>
       </c>
@@ -6270,7 +6264,7 @@
         <v>2022-12-01</v>
       </c>
       <c r="G16" s="33" t="str">
-        <f>IF(H16&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H16" s="34">
@@ -6299,7 +6293,7 @@
         <v>2022-12-02</v>
       </c>
       <c r="G17" s="33" t="str">
-        <f>IF(H17&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H17" s="34">
@@ -6328,7 +6322,7 @@
         <v>2022-12-05</v>
       </c>
       <c r="G18" s="33" t="str">
-        <f>IF(H18&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v>•</v>
       </c>
       <c r="H18" s="34">
@@ -6357,7 +6351,7 @@
         <v>2022-12-05</v>
       </c>
       <c r="G19" s="33" t="str">
-        <f>IF(H19&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H19" s="34">
@@ -6386,7 +6380,7 @@
         <v>2022-12-05</v>
       </c>
       <c r="G20" s="33" t="str">
-        <f>IF(H20&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H20" s="34">
@@ -6415,7 +6409,7 @@
         <v>2022-12-05</v>
       </c>
       <c r="G21" s="33" t="str">
-        <f>IF(H21&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H21" s="34">
@@ -6444,7 +6438,7 @@
         <v>2022-12-05</v>
       </c>
       <c r="G22" s="33" t="str">
-        <f>IF(H22&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H22" s="34">
@@ -6473,7 +6467,7 @@
         <v>2022-12-06</v>
       </c>
       <c r="G23" s="33" t="str">
-        <f>IF(H23&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H23" s="34">
@@ -6502,7 +6496,7 @@
         <v>2022-12-06</v>
       </c>
       <c r="G24" s="33" t="str">
-        <f>IF(H24&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H24" s="34">
@@ -6531,7 +6525,7 @@
         <v>2022-12-06</v>
       </c>
       <c r="G25" s="33" t="str">
-        <f>IF(H25&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H25" s="34">
@@ -6560,7 +6554,7 @@
         <v>2022-12-07</v>
       </c>
       <c r="G26" s="33" t="str">
-        <f>IF(H26&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H26" s="34">
@@ -6589,7 +6583,7 @@
         <v>2022-12-07</v>
       </c>
       <c r="G27" s="33" t="str">
-        <f>IF(H27&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v>•</v>
       </c>
       <c r="H27" s="34">
@@ -6618,7 +6612,7 @@
         <v>2022-12-07</v>
       </c>
       <c r="G28" s="33" t="str">
-        <f>IF(H28&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H28" s="34">
@@ -6647,7 +6641,7 @@
         <v>2022-12-07</v>
       </c>
       <c r="G29" s="33" t="str">
-        <f>IF(H29&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H29" s="34">
@@ -6676,7 +6670,7 @@
         <v>2022-12-08</v>
       </c>
       <c r="G30" s="33" t="str">
-        <f>IF(H30&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H30" s="34">
@@ -6705,7 +6699,7 @@
         <v>2022-12-08</v>
       </c>
       <c r="G31" s="33" t="str">
-        <f>IF(H31&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H31" s="34">
@@ -6734,7 +6728,7 @@
         <v>2022-12-08</v>
       </c>
       <c r="G32" s="33" t="str">
-        <f>IF(H32&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H32" s="34">
@@ -6763,7 +6757,7 @@
         <v>2022-12-08</v>
       </c>
       <c r="G33" s="33" t="str">
-        <f>IF(H33&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H33" s="34">
@@ -6792,7 +6786,7 @@
         <v>2022-12-09</v>
       </c>
       <c r="G34" s="33" t="str">
-        <f>IF(H34&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H34" s="34">
@@ -6821,7 +6815,7 @@
         <v>2022-12-09</v>
       </c>
       <c r="G35" s="33" t="str">
-        <f>IF(H35&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H35" s="34">
@@ -6850,7 +6844,7 @@
         <v>2022-12-09</v>
       </c>
       <c r="G36" s="33" t="str">
-        <f>IF(H36&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H36" s="34">
@@ -6879,7 +6873,7 @@
         <v>2022-12-12</v>
       </c>
       <c r="G37" s="33" t="str">
-        <f>IF(H37&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H37" s="34">
@@ -6908,7 +6902,7 @@
         <v>2022-12-12</v>
       </c>
       <c r="G38" s="33" t="str">
-        <f>IF(H38&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H38" s="34">
@@ -6937,7 +6931,7 @@
         <v>2022-12-13</v>
       </c>
       <c r="G39" s="33" t="str">
-        <f>IF(H39&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H39" s="34">
@@ -6966,7 +6960,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G40" s="33" t="str">
-        <f>IF(H40&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H40" s="34">
@@ -6995,7 +6989,7 @@
         <v>2022-12-15</v>
       </c>
       <c r="G41" s="33" t="str">
-        <f>IF(H41&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H41" s="34">
@@ -7024,7 +7018,7 @@
         <v>2022-12-15</v>
       </c>
       <c r="G42" s="33" t="str">
-        <f>IF(H42&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H42" s="34">
@@ -7053,7 +7047,7 @@
         <v>2022-12-16</v>
       </c>
       <c r="G43" s="33" t="str">
-        <f>IF(H43&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H43" s="34">
@@ -7082,7 +7076,7 @@
         <v>2022-12-19</v>
       </c>
       <c r="G44" s="33" t="str">
-        <f>IF(H44&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H44" s="34">
@@ -7111,7 +7105,7 @@
         <v>2022-12-21</v>
       </c>
       <c r="G45" s="33" t="str">
-        <f>IF(H45&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H45" s="34">
@@ -7140,7 +7134,7 @@
         <v>2022-12-21</v>
       </c>
       <c r="G46" s="33" t="str">
-        <f>IF(H46&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H46" s="34">
@@ -7169,7 +7163,7 @@
         <v>2022-12-23</v>
       </c>
       <c r="G47" s="33" t="str">
-        <f>IF(H47&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H47" s="34">
@@ -7198,7 +7192,7 @@
         <v>2022-12-26</v>
       </c>
       <c r="G48" s="33" t="str">
-        <f>IF(H48&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H48" s="34">
@@ -7227,7 +7221,7 @@
         <v>2022-12-26</v>
       </c>
       <c r="G49" s="33" t="str">
-        <f>IF(H49&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H49" s="34">
@@ -7256,7 +7250,7 @@
         <v>2023-01-06</v>
       </c>
       <c r="G50" s="33" t="str">
-        <f>IF(H50&gt;0,"•","")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="H50" s="34">
@@ -7295,7 +7289,7 @@
         <v>2022-11-21</v>
       </c>
       <c r="G52" s="33" t="str">
-        <f>IF(H52&gt;0,"•","")</f>
+        <f t="shared" ref="G52:G58" si="1">IF(H52&gt;0,"•","")</f>
         <v/>
       </c>
       <c r="H52" s="34">
@@ -7324,7 +7318,7 @@
         <v>2022-11-25</v>
       </c>
       <c r="G53" s="33" t="str">
-        <f>IF(H53&gt;0,"•","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H53" s="34">
@@ -7353,7 +7347,7 @@
         <v>2022-12-02</v>
       </c>
       <c r="G54" s="33" t="str">
-        <f>IF(H54&gt;0,"•","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H54" s="34">
@@ -7382,7 +7376,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G55" s="33" t="str">
-        <f>IF(H55&gt;0,"•","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H55" s="34">
@@ -7411,7 +7405,7 @@
         <v>2023-01-25</v>
       </c>
       <c r="G56" s="33" t="str">
-        <f>IF(H56&gt;0,"•","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H56" s="34">
@@ -7440,7 +7434,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="33" t="str">
-        <f>IF(H57&gt;0,"•","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H57" s="34">
@@ -7469,7 +7463,7 @@
         <v>0</v>
       </c>
       <c r="G58" s="33" t="str">
-        <f>IF(H58&gt;0,"•","")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H58" s="34">
@@ -7508,7 +7502,7 @@
         <v>2023-10-27</v>
       </c>
       <c r="G60" s="33" t="str">
-        <f>IF(H60&gt;0,"•","")</f>
+        <f t="shared" ref="G60:G103" si="2">IF(H60&gt;0,"•","")</f>
         <v/>
       </c>
       <c r="H60" s="34">
@@ -7537,7 +7531,7 @@
         <v>2022-11-25</v>
       </c>
       <c r="G61" s="33" t="str">
-        <f>IF(H61&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H61" s="34">
@@ -7566,7 +7560,7 @@
         <v>2022-11-25</v>
       </c>
       <c r="G62" s="33" t="str">
-        <f>IF(H62&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H62" s="34">
@@ -7595,7 +7589,7 @@
         <v>2022-12-02</v>
       </c>
       <c r="G63" s="33" t="str">
-        <f>IF(H63&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H63" s="34">
@@ -7624,7 +7618,7 @@
         <v>2022-12-02</v>
       </c>
       <c r="G64" s="33" t="str">
-        <f>IF(H64&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H64" s="34">
@@ -7653,7 +7647,7 @@
         <v>2022-12-02</v>
       </c>
       <c r="G65" s="33" t="str">
-        <f>IF(H65&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H65" s="34">
@@ -7682,7 +7676,7 @@
         <v>2022-12-07</v>
       </c>
       <c r="G66" s="33" t="str">
-        <f>IF(H66&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H66" s="34">
@@ -7711,7 +7705,7 @@
         <v>2022-12-08</v>
       </c>
       <c r="G67" s="33" t="str">
-        <f>IF(H67&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H67" s="34">
@@ -7740,7 +7734,7 @@
         <v>2022-12-09</v>
       </c>
       <c r="G68" s="33" t="str">
-        <f>IF(H68&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H68" s="34">
@@ -7769,7 +7763,7 @@
         <v>2022-12-09</v>
       </c>
       <c r="G69" s="33" t="str">
-        <f>IF(H69&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H69" s="34">
@@ -7798,7 +7792,7 @@
         <v>2022-12-12</v>
       </c>
       <c r="G70" s="33" t="str">
-        <f>IF(H70&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H70" s="34">
@@ -7827,7 +7821,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G71" s="33" t="str">
-        <f>IF(H71&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H71" s="34">
@@ -7856,7 +7850,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G72" s="33" t="str">
-        <f>IF(H72&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H72" s="34">
@@ -7885,7 +7879,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G73" s="33" t="str">
-        <f>IF(H73&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H73" s="34">
@@ -7914,7 +7908,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G74" s="33" t="str">
-        <f>IF(H74&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H74" s="34">
@@ -7943,7 +7937,7 @@
         <v>2022-12-15</v>
       </c>
       <c r="G75" s="33" t="str">
-        <f>IF(H75&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H75" s="34">
@@ -7972,7 +7966,7 @@
         <v>2022-12-16</v>
       </c>
       <c r="G76" s="33" t="str">
-        <f>IF(H76&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H76" s="34">
@@ -8001,7 +7995,7 @@
         <v>2022-12-16</v>
       </c>
       <c r="G77" s="33" t="str">
-        <f>IF(H77&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H77" s="34">
@@ -8030,7 +8024,7 @@
         <v>2022-12-19</v>
       </c>
       <c r="G78" s="33" t="str">
-        <f>IF(H78&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H78" s="34">
@@ -8059,7 +8053,7 @@
         <v>2022-12-20</v>
       </c>
       <c r="G79" s="33" t="str">
-        <f>IF(H79&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H79" s="34">
@@ -8088,7 +8082,7 @@
         <v>2022-12-21</v>
       </c>
       <c r="G80" s="33" t="str">
-        <f>IF(H80&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H80" s="34">
@@ -8117,7 +8111,7 @@
         <v>2022-12-23</v>
       </c>
       <c r="G81" s="33" t="str">
-        <f>IF(H81&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H81" s="34">
@@ -8146,7 +8140,7 @@
         <v>2022-12-23</v>
       </c>
       <c r="G82" s="33" t="str">
-        <f>IF(H82&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H82" s="34">
@@ -8175,7 +8169,7 @@
         <v>2022-12-27</v>
       </c>
       <c r="G83" s="33" t="str">
-        <f>IF(H83&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H83" s="34">
@@ -8204,7 +8198,7 @@
         <v>2022-12-27</v>
       </c>
       <c r="G84" s="33" t="str">
-        <f>IF(H84&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H84" s="34">
@@ -8233,7 +8227,7 @@
         <v>2022-12-27</v>
       </c>
       <c r="G85" s="33" t="str">
-        <f>IF(H85&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H85" s="34">
@@ -8262,7 +8256,7 @@
         <v>2022-12-28</v>
       </c>
       <c r="G86" s="33" t="str">
-        <f>IF(H86&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H86" s="34">
@@ -8291,7 +8285,7 @@
         <v>2022-12-29</v>
       </c>
       <c r="G87" s="33" t="str">
-        <f>IF(H87&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H87" s="34">
@@ -8320,7 +8314,7 @@
         <v>2023-01-03</v>
       </c>
       <c r="G88" s="33" t="str">
-        <f>IF(H88&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H88" s="34">
@@ -8349,7 +8343,7 @@
         <v>2023-01-04</v>
       </c>
       <c r="G89" s="33" t="str">
-        <f>IF(H89&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H89" s="34">
@@ -8378,7 +8372,7 @@
         <v>2023-01-10</v>
       </c>
       <c r="G90" s="33" t="str">
-        <f>IF(H90&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H90" s="34">
@@ -8407,7 +8401,7 @@
         <v>2023-01-16</v>
       </c>
       <c r="G91" s="33" t="str">
-        <f>IF(H91&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H91" s="34">
@@ -8436,7 +8430,7 @@
         <v>2023-01-16</v>
       </c>
       <c r="G92" s="33" t="str">
-        <f>IF(H92&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H92" s="34">
@@ -8465,7 +8459,7 @@
         <v>2023-01-16</v>
       </c>
       <c r="G93" s="33" t="str">
-        <f>IF(H93&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H93" s="34">
@@ -8494,7 +8488,7 @@
         <v>2023-01-17</v>
       </c>
       <c r="G94" s="33" t="str">
-        <f>IF(H94&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H94" s="34">
@@ -8523,7 +8517,7 @@
         <v>2023-01-24</v>
       </c>
       <c r="G95" s="33" t="str">
-        <f>IF(H95&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H95" s="34">
@@ -8552,7 +8546,7 @@
         <v>2023-01-26</v>
       </c>
       <c r="G96" s="33" t="str">
-        <f>IF(H96&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H96" s="34">
@@ -8581,7 +8575,7 @@
         <v>2023-01-27</v>
       </c>
       <c r="G97" s="33" t="str">
-        <f>IF(H97&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v>•</v>
       </c>
       <c r="H97" s="34">
@@ -8610,7 +8604,7 @@
         <v>2023-02-13</v>
       </c>
       <c r="G98" s="33" t="str">
-        <f>IF(H98&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H98" s="34">
@@ -8639,7 +8633,7 @@
         <v>2023-02-27</v>
       </c>
       <c r="G99" s="33" t="str">
-        <f>IF(H99&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H99" s="34">
@@ -8668,7 +8662,7 @@
         <v>2023-07-20</v>
       </c>
       <c r="G100" s="33" t="str">
-        <f>IF(H100&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H100" s="34">
@@ -8697,7 +8691,7 @@
         <v>2023-08-14</v>
       </c>
       <c r="G101" s="33" t="str">
-        <f>IF(H101&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H101" s="34">
@@ -8726,7 +8720,7 @@
         <v>2023-08-15</v>
       </c>
       <c r="G102" s="33" t="str">
-        <f>IF(H102&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H102" s="34">
@@ -8755,7 +8749,7 @@
         <v>2023-08-24</v>
       </c>
       <c r="G103" s="33" t="str">
-        <f>IF(H103&gt;0,"•","")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="H103" s="34">
@@ -8794,7 +8788,7 @@
         <v>2022-11-16</v>
       </c>
       <c r="G105" s="33" t="str">
-        <f>IF(H105&gt;0,"•","")</f>
+        <f t="shared" ref="G105:G113" si="3">IF(H105&gt;0,"•","")</f>
         <v>•</v>
       </c>
       <c r="H105" s="34">
@@ -8823,7 +8817,7 @@
         <v>2022-11-21</v>
       </c>
       <c r="G106" s="33" t="str">
-        <f>IF(H106&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v>•</v>
       </c>
       <c r="H106" s="34">
@@ -8852,7 +8846,7 @@
         <v>2022-11-23</v>
       </c>
       <c r="G107" s="33" t="str">
-        <f>IF(H107&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H107" s="34">
@@ -8881,7 +8875,7 @@
         <v>2022-11-30</v>
       </c>
       <c r="G108" s="33" t="str">
-        <f>IF(H108&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H108" s="34">
@@ -8910,7 +8904,7 @@
         <v>2022-12-01</v>
       </c>
       <c r="G109" s="33" t="str">
-        <f>IF(H109&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H109" s="34">
@@ -8939,7 +8933,7 @@
         <v>2022-12-01</v>
       </c>
       <c r="G110" s="33" t="str">
-        <f>IF(H110&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H110" s="34">
@@ -8968,7 +8962,7 @@
         <v>2022-12-02</v>
       </c>
       <c r="G111" s="33" t="str">
-        <f>IF(H111&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H111" s="34">
@@ -8997,7 +8991,7 @@
         <v>2022-12-06</v>
       </c>
       <c r="G112" s="33" t="str">
-        <f>IF(H112&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H112" s="34">
@@ -9026,7 +9020,7 @@
         <v>2022-12-14</v>
       </c>
       <c r="G113" s="33" t="str">
-        <f>IF(H113&gt;0,"•","")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="H113" s="34">
@@ -9078,8 +9072,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
-  <sortState ref="A105:J113">
-    <sortCondition ref="B105:B113"/>
+  <sortState ref="A60:E103">
+    <sortCondition ref="B60:B103"/>
   </sortState>
   <conditionalFormatting sqref="B3">
     <cfRule type="iconSet" priority="31">

</xml_diff>